<commit_message>
b4 dp on 7
</commit_message>
<xml_diff>
--- a/result/boringssl_total2_tmp10.xlsx
+++ b/result/boringssl_total2_tmp10.xlsx
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8589762501843929</v>
+        <v>0.8282101349795783</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6726542871169896</v>
+        <v>0.8013695804628522</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7544822894903066</v>
+        <v>0.8145688144178597</v>
       </c>
       <c r="E2" t="n">
-        <v>242389</v>
+        <v>242410</v>
       </c>
     </row>
     <row r="3">
@@ -503,10 +503,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8882175226586103</v>
+        <v>0.918429003021148</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9408000000000001</v>
+        <v>0.95748031496063</v>
       </c>
       <c r="E4" t="n">
         <v>331</v>
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7237781986112496</v>
+        <v>0.9253686759110775</v>
       </c>
       <c r="C5" t="n">
-        <v>0.739502359211107</v>
+        <v>0.6661724426737895</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7315557943517245</v>
+        <v>0.7746643853645695</v>
       </c>
       <c r="E5" t="n">
-        <v>88377</v>
+        <v>88354</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8990509059534081</v>
+        <v>0.6012188154637212</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9856534762730569</v>
+        <v>0.9955849889624724</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9403624877791984</v>
+        <v>0.7497031583946806</v>
       </c>
       <c r="E6" t="n">
-        <v>6343</v>
+        <v>6342</v>
       </c>
     </row>
     <row r="7">
@@ -557,16 +557,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8916123547747237</v>
+        <v>0.9869396968719768</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9919609079445145</v>
+        <v>0.9645445950204854</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9391135651395315</v>
+        <v>0.9756136436085432</v>
       </c>
       <c r="E7" t="n">
-        <v>6344</v>
+        <v>6346</v>
       </c>
     </row>
     <row r="8">
@@ -576,16 +576,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4564568513986414</v>
+        <v>0.9732906848057873</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9628499402945468</v>
+        <v>0.8699244855123164</v>
       </c>
       <c r="D8" t="n">
-        <v>0.619315647171546</v>
+        <v>0.9187092335915206</v>
       </c>
       <c r="E8" t="n">
-        <v>82907</v>
+        <v>82898</v>
       </c>
     </row>
     <row r="9">
@@ -595,16 +595,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9431336509246409</v>
+        <v>0.9449248120300752</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9097586568730325</v>
+        <v>0.9701706772812255</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9261455724178577</v>
+        <v>0.9573813420621931</v>
       </c>
       <c r="E9" t="n">
-        <v>82911</v>
+        <v>82905</v>
       </c>
     </row>
     <row r="10">
@@ -614,13 +614,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9567263614693479</v>
+        <v>0.2961875722050719</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9343401181877873</v>
+        <v>0.9335044469647228</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9454007368484628</v>
+        <v>0.4496937631193029</v>
       </c>
       <c r="E10" t="n">
         <v>16753</v>
@@ -633,16 +633,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.8773868796848499</v>
+        <v>0.8952116191989107</v>
       </c>
       <c r="C11" t="n">
-        <v>0.957258834765998</v>
+        <v>0.9415239572766871</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9155842302092552</v>
+        <v>0.9177839174058455</v>
       </c>
       <c r="E11" t="n">
-        <v>16752</v>
+        <v>16759</v>
       </c>
     </row>
     <row r="12">
@@ -652,16 +652,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.6436504104297441</v>
+        <v>0.6563146997929606</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2051084782274196</v>
+        <v>0.1951970443349754</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3110851808634773</v>
+        <v>0.3009017560512577</v>
       </c>
       <c r="E12" t="n">
-        <v>6499</v>
+        <v>6496</v>
       </c>
     </row>
     <row r="13">
@@ -690,16 +690,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.6170770633834929</v>
+        <v>0.525649145028499</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7254087376038596</v>
+        <v>0.667291973737103</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6668719970432426</v>
+        <v>0.5880616401960205</v>
       </c>
       <c r="E14" t="n">
-        <v>7462</v>
+        <v>7463</v>
       </c>
     </row>
     <row r="15">
@@ -709,16 +709,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.5295358649789029</v>
+        <v>0.3909877105143377</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6141924959216966</v>
+        <v>0.701797385620915</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5687311178247735</v>
+        <v>0.5021923414206372</v>
       </c>
       <c r="E15" t="n">
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="16">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.7906976744186046</v>
+        <v>0.7192982456140351</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2297297297297297</v>
+        <v>0.2789115646258503</v>
       </c>
       <c r="D16" t="n">
-        <v>0.356020942408377</v>
+        <v>0.4019607843137255</v>
       </c>
       <c r="E16" t="n">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17">
@@ -747,16 +747,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9209458911332846</v>
+        <v>0.7517265747968264</v>
       </c>
       <c r="C17" t="n">
-        <v>0.854631685926149</v>
+        <v>0.880834086118639</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8865504382967923</v>
+        <v>0.8111752370058408</v>
       </c>
       <c r="E17" t="n">
-        <v>26567</v>
+        <v>26568</v>
       </c>
     </row>
     <row r="18">
@@ -766,13 +766,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.06818181818181818</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0.08333333333333333</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.075</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
         <v>36</v>
@@ -785,16 +785,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.2512471655328798</v>
+        <v>0.1976796073181615</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2030047636496885</v>
+        <v>0.1621522693997072</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2245642480745845</v>
+        <v>0.178162075206113</v>
       </c>
       <c r="E19" t="n">
-        <v>2729</v>
+        <v>2732</v>
       </c>
     </row>
     <row r="20">
@@ -804,13 +804,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.7626876340243031</v>
+        <v>0.7486522911051213</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6937581274382315</v>
+        <v>0.7223667100130039</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7265917602996255</v>
+        <v>0.7352746525479815</v>
       </c>
       <c r="E20" t="n">
         <v>1538</v>
@@ -823,16 +823,16 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.5343601895734598</v>
+        <v>0.5646153846153846</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4295238095238095</v>
+        <v>0.3491912464319695</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4762407602956705</v>
+        <v>0.4315108759553204</v>
       </c>
       <c r="E21" t="n">
-        <v>1050</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="22">
@@ -842,16 +842,16 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.6679723201462332</v>
+        <v>0.4668217775709632</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7504767493032125</v>
+        <v>0.7355917289925209</v>
       </c>
       <c r="D22" t="n">
-        <v>0.7068250898038132</v>
+        <v>0.5711682987929857</v>
       </c>
       <c r="E22" t="n">
-        <v>6817</v>
+        <v>6819</v>
       </c>
     </row>
     <row r="23">
@@ -861,16 +861,16 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.7762499246125083</v>
+        <v>0.8085913259325657</v>
       </c>
       <c r="C23" t="n">
-        <v>0.8396503359645117</v>
+        <v>0.7647710969088301</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8067063616421185</v>
+        <v>0.7860709856889098</v>
       </c>
       <c r="E23" t="n">
-        <v>15329</v>
+        <v>15334</v>
       </c>
     </row>
     <row r="24">
@@ -880,13 +880,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.6559139784946236</v>
+        <v>0.7884615384615384</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1826347305389222</v>
+        <v>0.1227544910179641</v>
       </c>
       <c r="D24" t="n">
-        <v>0.2857142857142858</v>
+        <v>0.2124352331606218</v>
       </c>
       <c r="E24" t="n">
         <v>334</v>
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="26">
@@ -918,13 +918,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.8970588235294118</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C26" t="n">
-        <v>0.2074829931972789</v>
+        <v>0.2448979591836735</v>
       </c>
       <c r="D26" t="n">
-        <v>0.3370165745856353</v>
+        <v>0.3582089552238806</v>
       </c>
       <c r="E26" t="n">
         <v>294</v>
@@ -937,16 +937,16 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.9609414121181773</v>
+        <v>0.9713045575114541</v>
       </c>
       <c r="C27" t="n">
-        <v>0.8971482000935016</v>
+        <v>0.9413414349146997</v>
       </c>
       <c r="D27" t="n">
-        <v>0.9279497098646036</v>
+        <v>0.9560882981248516</v>
       </c>
       <c r="E27" t="n">
-        <v>4278</v>
+        <v>4279</v>
       </c>
     </row>
     <row r="28">
@@ -956,16 +956,16 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.472463768115942</v>
+        <v>0.4606275902901125</v>
       </c>
       <c r="C28" t="n">
-        <v>0.3732112192329708</v>
+        <v>0.4445714285714286</v>
       </c>
       <c r="D28" t="n">
-        <v>0.4170131116085705</v>
+        <v>0.4524571096248909</v>
       </c>
       <c r="E28" t="n">
-        <v>1747</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="29">
@@ -975,13 +975,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.2428571428571429</v>
+        <v>0.1262376237623762</v>
       </c>
       <c r="C29" t="n">
         <v>0.1526946107784431</v>
       </c>
       <c r="D29" t="n">
-        <v>0.1875</v>
+        <v>0.1382113821138211</v>
       </c>
       <c r="E29" t="n">
         <v>334</v>
@@ -1013,16 +1013,16 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>4.459308807134894e-05</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>8.918219923303309e-05</v>
       </c>
       <c r="E31" t="n">
-        <v>44854</v>
+        <v>44850</v>
       </c>
     </row>
     <row r="32">
@@ -1051,16 +1051,16 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.434010152284264</v>
+        <v>0.39786156443444</v>
       </c>
       <c r="C33" t="n">
-        <v>0.5285935085007728</v>
+        <v>0.5467904098994586</v>
       </c>
       <c r="D33" t="n">
-        <v>0.4766550522648084</v>
+        <v>0.460586319218241</v>
       </c>
       <c r="E33" t="n">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="34">
@@ -1070,16 +1070,16 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.4373544480670704</v>
+        <v>0.4055220017256255</v>
       </c>
       <c r="C34" t="n">
-        <v>0.5266404935501963</v>
+        <v>0.5280898876404494</v>
       </c>
       <c r="D34" t="n">
-        <v>0.4778625954198473</v>
+        <v>0.4587603709126403</v>
       </c>
       <c r="E34" t="n">
-        <v>1783</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="35">
@@ -1089,13 +1089,13 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.8611111111111112</v>
+        <v>0.8958333333333334</v>
       </c>
       <c r="C35" t="n">
-        <v>0.04754601226993865</v>
+        <v>0.06595092024539877</v>
       </c>
       <c r="D35" t="n">
-        <v>0.09011627906976744</v>
+        <v>0.1228571428571428</v>
       </c>
       <c r="E35" t="n">
         <v>652</v>
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.2543604651162791</v>
+        <v>0.3799126637554585</v>
       </c>
       <c r="C37" t="n">
-        <v>0.2198492462311558</v>
+        <v>0.2188679245283019</v>
       </c>
       <c r="D37" t="n">
-        <v>0.2358490566037736</v>
+        <v>0.277733439744613</v>
       </c>
       <c r="E37" t="n">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="38">
@@ -1146,13 +1146,13 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.7837116154873164</v>
+        <v>0.8944099378881988</v>
       </c>
       <c r="C38" t="n">
-        <v>0.3570559610705596</v>
+        <v>0.1751824817518248</v>
       </c>
       <c r="D38" t="n">
-        <v>0.4905975762641036</v>
+        <v>0.2929806714140386</v>
       </c>
       <c r="E38" t="n">
         <v>1644</v>
@@ -1165,16 +1165,16 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.4296875</v>
       </c>
       <c r="C39" t="n">
-        <v>0.1364829396325459</v>
+        <v>0.143979057591623</v>
       </c>
       <c r="D39" t="n">
-        <v>0.2180293501048218</v>
+        <v>0.2156862745098039</v>
       </c>
       <c r="E39" t="n">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="40">
@@ -1241,13 +1241,13 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.4880952380952381</v>
+        <v>0.4979955456570156</v>
       </c>
       <c r="C43" t="n">
-        <v>0.3262599469496021</v>
+        <v>0.4942528735632184</v>
       </c>
       <c r="D43" t="n">
-        <v>0.3910969793322734</v>
+        <v>0.4961171510982915</v>
       </c>
       <c r="E43" t="n">
         <v>2262</v>
@@ -1260,16 +1260,16 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.8367491166077738</v>
+        <v>0.8875638841567292</v>
       </c>
       <c r="C44" t="n">
-        <v>0.6277836691410392</v>
+        <v>0.5516146109052409</v>
       </c>
       <c r="D44" t="n">
-        <v>0.7173583762496214</v>
+        <v>0.6803787136793992</v>
       </c>
       <c r="E44" t="n">
-        <v>1886</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="45">
@@ -1279,13 +1279,13 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.1016949152542373</v>
+        <v>0.03092783505154639</v>
       </c>
       <c r="C45" t="n">
-        <v>0.04137931034482759</v>
+        <v>0.006896551724137931</v>
       </c>
       <c r="D45" t="n">
-        <v>0.05882352941176471</v>
+        <v>0.0112781954887218</v>
       </c>
       <c r="E45" t="n">
         <v>435</v>
@@ -1298,13 +1298,13 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.4550324217648717</v>
+        <v>0.3619456366237482</v>
       </c>
       <c r="C46" t="n">
-        <v>0.9799635701275046</v>
+        <v>0.4608378870673953</v>
       </c>
       <c r="D46" t="n">
-        <v>0.6214863303812092</v>
+        <v>0.405448717948718</v>
       </c>
       <c r="E46" t="n">
         <v>1647</v>
@@ -1317,13 +1317,13 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.857188498402556</v>
+        <v>0.8804845222072678</v>
       </c>
       <c r="C47" t="n">
-        <v>0.5363854458216714</v>
+        <v>0.653938424630148</v>
       </c>
       <c r="D47" t="n">
-        <v>0.6598622725036892</v>
+        <v>0.7504875530572445</v>
       </c>
       <c r="E47" t="n">
         <v>5002</v>
@@ -1336,16 +1336,16 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.855637883930789</v>
+        <v>0.8566384760653584</v>
       </c>
       <c r="C48" t="n">
-        <v>0.9732790281570769</v>
+        <v>0.9826693039465009</v>
       </c>
       <c r="D48" t="n">
-        <v>0.9106749493347431</v>
+        <v>0.9153360238638356</v>
       </c>
       <c r="E48" t="n">
-        <v>42476</v>
+        <v>42468</v>
       </c>
     </row>
     <row r="49">
@@ -1355,16 +1355,16 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.8103821587095378</v>
+        <v>0.771246203737067</v>
       </c>
       <c r="C49" t="n">
-        <v>0.9393863336889</v>
+        <v>0.9401982931726908</v>
       </c>
       <c r="D49" t="n">
-        <v>0.8701287379035774</v>
+        <v>0.8473828577892147</v>
       </c>
       <c r="E49" t="n">
-        <v>15937</v>
+        <v>15936</v>
       </c>
     </row>
     <row r="50">
@@ -1374,13 +1374,13 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.4895497026338148</v>
+        <v>0.5083210059171598</v>
       </c>
       <c r="C50" t="n">
-        <v>0.8156851642129105</v>
+        <v>0.7783125707814269</v>
       </c>
       <c r="D50" t="n">
-        <v>0.6118721461187214</v>
+        <v>0.6149888143176733</v>
       </c>
       <c r="E50" t="n">
         <v>3532</v>
@@ -1393,16 +1393,16 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.7562610904984675</v>
+        <v>0.6043496318670946</v>
       </c>
       <c r="C51" t="n">
-        <v>0.7673476486174055</v>
+        <v>0.8187314578005115</v>
       </c>
       <c r="D51" t="n">
-        <v>0.761764033818265</v>
+        <v>0.6953926360377973</v>
       </c>
       <c r="E51" t="n">
-        <v>97751</v>
+        <v>97750</v>
       </c>
     </row>
     <row r="52">
@@ -1412,16 +1412,16 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.1181938911022576</v>
+        <v>0.4340044742729307</v>
       </c>
       <c r="C52" t="n">
-        <v>0.7911111111111111</v>
+        <v>0.8584070796460177</v>
       </c>
       <c r="D52" t="n">
-        <v>0.2056614673599076</v>
+        <v>0.5765230312035661</v>
       </c>
       <c r="E52" t="n">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="53">
@@ -1450,16 +1450,16 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.8342618384401114</v>
+        <v>0.897887323943662</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9089529590288316</v>
+        <v>0.7727272727272727</v>
       </c>
       <c r="D54" t="n">
-        <v>0.8700072621641249</v>
+        <v>0.8306188925081434</v>
       </c>
       <c r="E54" t="n">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="55">
@@ -1469,16 +1469,16 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.7908961593172119</v>
+        <v>0.9770354906054279</v>
       </c>
       <c r="C55" t="n">
-        <v>0.9937444146559428</v>
+        <v>0.8349687778768956</v>
       </c>
       <c r="D55" t="n">
-        <v>0.8807920792079207</v>
+        <v>0.9004329004329005</v>
       </c>
       <c r="E55" t="n">
-        <v>1119</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="56">
@@ -1488,13 +1488,13 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.4273921200750469</v>
+        <v>0.5219421101774043</v>
       </c>
       <c r="C56" t="n">
-        <v>0.5957112970711297</v>
+        <v>0.5847280334728033</v>
       </c>
       <c r="D56" t="n">
-        <v>0.4977059209088923</v>
+        <v>0.5515540207202764</v>
       </c>
       <c r="E56" t="n">
         <v>1912</v>
@@ -1507,16 +1507,16 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.4762776291707729</v>
+        <v>0.5328445308992967</v>
       </c>
       <c r="C57" t="n">
-        <v>0.7061156334794406</v>
+        <v>0.7428035043804756</v>
       </c>
       <c r="D57" t="n">
-        <v>0.5688582478560619</v>
+        <v>0.620545438703494</v>
       </c>
       <c r="E57" t="n">
-        <v>4791</v>
+        <v>4794</v>
       </c>
     </row>
     <row r="58">
@@ -1526,13 +1526,13 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0</v>
+        <v>0.2346368715083799</v>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>0.3122676579925651</v>
       </c>
       <c r="E58" t="n">
         <v>90</v>
@@ -1545,16 +1545,16 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.8363636363636363</v>
+        <v>1</v>
       </c>
       <c r="C59" t="n">
-        <v>0.9019607843137255</v>
+        <v>0.495049504950495</v>
       </c>
       <c r="D59" t="n">
-        <v>0.8679245283018867</v>
+        <v>0.6622516556291391</v>
       </c>
       <c r="E59" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60">
@@ -1564,13 +1564,13 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.7673267326732673</v>
+        <v>0.6926229508196722</v>
       </c>
       <c r="C60" t="n">
-        <v>0.856353591160221</v>
+        <v>0.9337016574585635</v>
       </c>
       <c r="D60" t="n">
-        <v>0.8093994778067886</v>
+        <v>0.7952941176470588</v>
       </c>
       <c r="E60" t="n">
         <v>181</v>
@@ -1602,13 +1602,13 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.8325053229240597</v>
+        <v>0.8458702064896755</v>
       </c>
       <c r="C62" t="n">
-        <v>0.8078512396694215</v>
+        <v>0.7899449035812672</v>
       </c>
       <c r="D62" t="n">
-        <v>0.8199930094372596</v>
+        <v>0.816951566951567</v>
       </c>
       <c r="E62" t="n">
         <v>1452</v>
@@ -1640,13 +1640,13 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="E64" t="n">
         <v>25</v>
@@ -1678,16 +1678,16 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.949874686716792</v>
+        <v>0.9986876640419947</v>
       </c>
       <c r="C66" t="n">
-        <v>0.9869791666666666</v>
+        <v>0.9870298313878081</v>
       </c>
       <c r="D66" t="n">
-        <v>0.9680715197956578</v>
+        <v>0.9928245270711025</v>
       </c>
       <c r="E66" t="n">
-        <v>768</v>
+        <v>771</v>
       </c>
     </row>
     <row r="67">
@@ -1697,16 +1697,16 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.9150253235790659</v>
+        <v>0.952638700947226</v>
       </c>
       <c r="C67" t="n">
-        <v>0.6580331849453662</v>
+        <v>0.5709651257096513</v>
       </c>
       <c r="D67" t="n">
-        <v>0.7655367231638418</v>
+        <v>0.7139959432048681</v>
       </c>
       <c r="E67" t="n">
-        <v>2471</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="68">
@@ -1716,16 +1716,16 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.9341400332532791</v>
+        <v>0.9058646082867536</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9859608072535829</v>
+        <v>0.9953207252875804</v>
       </c>
       <c r="D68" t="n">
-        <v>0.9593511359863397</v>
+        <v>0.9484880858377073</v>
       </c>
       <c r="E68" t="n">
-        <v>10257</v>
+        <v>10258</v>
       </c>
     </row>
     <row r="69">
@@ -1735,13 +1735,13 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4</v>
       </c>
       <c r="C69" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="D69" t="n">
-        <v>0.6956521739130435</v>
+        <v>0.2500000000000001</v>
       </c>
       <c r="E69" t="n">
         <v>11</v>
@@ -1754,16 +1754,16 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.5019441069258809</v>
+        <v>0.6107406739953145</v>
       </c>
       <c r="C70" t="n">
-        <v>0.7970287478294424</v>
+        <v>0.6537422839506173</v>
       </c>
       <c r="D70" t="n">
-        <v>0.6159695817490494</v>
+        <v>0.6315102953507873</v>
       </c>
       <c r="E70" t="n">
-        <v>5183</v>
+        <v>5184</v>
       </c>
     </row>
     <row r="71">
@@ -1773,16 +1773,16 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.2434782608695652</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="C71" t="n">
-        <v>0.02280130293159609</v>
+        <v>0.005695687550854353</v>
       </c>
       <c r="D71" t="n">
-        <v>0.04169769173492182</v>
+        <v>0.01129032258064516</v>
       </c>
       <c r="E71" t="n">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="72">
@@ -1811,16 +1811,16 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.8130099474684251</v>
+        <v>0.8155170408281959</v>
       </c>
       <c r="C73" t="n">
-        <v>0.943450064850843</v>
+        <v>0.9091026970954357</v>
       </c>
       <c r="D73" t="n">
-        <v>0.8733865642072401</v>
+        <v>0.8597706787663253</v>
       </c>
       <c r="E73" t="n">
-        <v>7710</v>
+        <v>7712</v>
       </c>
     </row>
     <row r="74">
@@ -1830,13 +1830,13 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.75</v>
+        <v>0.84</v>
       </c>
       <c r="C74" t="n">
         <v>0.875</v>
       </c>
       <c r="D74" t="n">
-        <v>0.8076923076923077</v>
+        <v>0.8571428571428572</v>
       </c>
       <c r="E74" t="n">
         <v>24</v>
@@ -1868,16 +1868,16 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.4663787785317705</v>
+        <v>0.5709057639524245</v>
       </c>
       <c r="C76" t="n">
-        <v>0.7125353440150801</v>
+        <v>0.5875706214689266</v>
       </c>
       <c r="D76" t="n">
-        <v>0.5637583892617449</v>
+        <v>0.5791183294663573</v>
       </c>
       <c r="E76" t="n">
-        <v>1061</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="77">
@@ -1887,16 +1887,16 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.7202158572021585</v>
+        <v>0.8228516562650025</v>
       </c>
       <c r="C77" t="n">
-        <v>0.9268162393162394</v>
+        <v>0.9151094500800854</v>
       </c>
       <c r="D77" t="n">
-        <v>0.8105582807755197</v>
+        <v>0.8665318503538929</v>
       </c>
       <c r="E77" t="n">
-        <v>1872</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="78">
@@ -1906,13 +1906,13 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.3291703835860839</v>
+        <v>0.1899736147757256</v>
       </c>
       <c r="C78" t="n">
-        <v>0.2450199203187251</v>
+        <v>0.2390438247011952</v>
       </c>
       <c r="D78" t="n">
-        <v>0.2809288161400837</v>
+        <v>0.2117024404586886</v>
       </c>
       <c r="E78" t="n">
         <v>1506</v>
@@ -1925,13 +1925,13 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.6507177033492823</v>
+        <v>0.6787564766839378</v>
       </c>
       <c r="C79" t="n">
-        <v>0.9251700680272109</v>
+        <v>0.891156462585034</v>
       </c>
       <c r="D79" t="n">
-        <v>0.7640449438202247</v>
+        <v>0.7705882352941176</v>
       </c>
       <c r="E79" t="n">
         <v>147</v>
@@ -1944,16 +1944,16 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.5816326530612245</v>
+        <v>0.8627450980392157</v>
       </c>
       <c r="C80" t="n">
-        <v>0.7215189873417721</v>
+        <v>0.5641025641025641</v>
       </c>
       <c r="D80" t="n">
-        <v>0.6440677966101694</v>
+        <v>0.682170542635659</v>
       </c>
       <c r="E80" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81">
@@ -1963,13 +1963,13 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>0.07407407407407407</v>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>0.1379310344827586</v>
       </c>
       <c r="E81" t="n">
         <v>27</v>
@@ -1982,16 +1982,16 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.8936781609195402</v>
+        <v>0.8775029446407538</v>
       </c>
       <c r="C82" t="n">
-        <v>0.386335403726708</v>
+        <v>0.4630205096333126</v>
       </c>
       <c r="D82" t="n">
-        <v>0.5394622723330442</v>
+        <v>0.6061838893409276</v>
       </c>
       <c r="E82" t="n">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="83">
@@ -2001,16 +2001,16 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.8806572499279332</v>
+        <v>0.8427738172391446</v>
       </c>
       <c r="C83" t="n">
-        <v>0.7634637011120829</v>
+        <v>0.8121408943292531</v>
       </c>
       <c r="D83" t="n">
-        <v>0.8178836757914463</v>
+        <v>0.8271738439030596</v>
       </c>
       <c r="E83" t="n">
-        <v>8003</v>
+        <v>8006</v>
       </c>
     </row>
     <row r="84">
@@ -2020,13 +2020,13 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="D84" t="n">
-        <v>0.2222222222222222</v>
+        <v>0</v>
       </c>
       <c r="E84" t="n">
         <v>8</v>
@@ -2039,16 +2039,16 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.6506849315068494</v>
+        <v>0.6075949367088608</v>
       </c>
       <c r="C85" t="n">
-        <v>0.4702970297029703</v>
+        <v>0.4740740740740741</v>
       </c>
       <c r="D85" t="n">
-        <v>0.5459770114942528</v>
+        <v>0.5325936199722608</v>
       </c>
       <c r="E85" t="n">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="86">
@@ -2115,16 +2115,16 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.9787234042553191</v>
+        <v>1</v>
       </c>
       <c r="C89" t="n">
-        <v>0.1345029239766082</v>
+        <v>0.01744186046511628</v>
       </c>
       <c r="D89" t="n">
-        <v>0.2365038560411311</v>
+        <v>0.03428571428571429</v>
       </c>
       <c r="E89" t="n">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="90">
@@ -2134,13 +2134,13 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.64</v>
+        <v>0.6805555555555556</v>
       </c>
       <c r="C90" t="n">
-        <v>0.4067796610169492</v>
+        <v>0.4152542372881356</v>
       </c>
       <c r="D90" t="n">
-        <v>0.4974093264248705</v>
+        <v>0.5157894736842105</v>
       </c>
       <c r="E90" t="n">
         <v>118</v>
@@ -2172,13 +2172,13 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.4615384615384616</v>
       </c>
       <c r="C92" t="n">
-        <v>0.1344086021505376</v>
+        <v>0.3548387096774194</v>
       </c>
       <c r="D92" t="n">
-        <v>0.2262443438914027</v>
+        <v>0.4012158054711246</v>
       </c>
       <c r="E92" t="n">
         <v>186</v>
@@ -2187,7 +2187,7 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>163.0</t>
+          <t>162.0</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -2200,13 +2200,13 @@
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>164.0</t>
+          <t>163.0</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -2219,13 +2219,13 @@
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>165.0</t>
+          <t>164.0</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -2238,13 +2238,13 @@
         <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>168.0</t>
+          <t>165.0</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -2257,23 +2257,23 @@
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>169.0</t>
+          <t>168.0</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="C97" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D97" t="n">
-        <v>0.4615384615384615</v>
+        <v>0.4</v>
       </c>
       <c r="E97" t="n">
         <v>12</v>
@@ -2282,64 +2282,64 @@
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>170.0</t>
+          <t>169.0</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D98" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E98" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>173.0</t>
+          <t>170.0</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.1896551724137931</v>
+        <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>0.2588235294117647</v>
+        <v>0</v>
       </c>
       <c r="D99" t="n">
-        <v>0.2189054726368159</v>
+        <v>0</v>
       </c>
       <c r="E99" t="n">
-        <v>85</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>175.0</t>
+          <t>173.0</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0</v>
+        <v>0.3269230769230769</v>
       </c>
       <c r="C100" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>0.2481751824817518</v>
       </c>
       <c r="E100" t="n">
-        <v>2</v>
+        <v>85</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>177.0</t>
+          <t>175.0</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -2352,7 +2352,7 @@
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
@@ -2381,13 +2381,13 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.6934235976789168</v>
+        <v>0.7332704995287465</v>
       </c>
       <c r="C103" t="n">
-        <v>0.6789772727272727</v>
+        <v>0.7367424242424242</v>
       </c>
       <c r="D103" t="n">
-        <v>0.6861244019138755</v>
+        <v>0.7350023618327822</v>
       </c>
       <c r="E103" t="n">
         <v>1056</v>
@@ -2400,16 +2400,16 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.7405238095238095</v>
+        <v>0.768202657807309</v>
       </c>
       <c r="C104" t="n">
-        <v>0.7405238095238095</v>
+        <v>0.768202657807309</v>
       </c>
       <c r="D104" t="n">
-        <v>0.7405238095238095</v>
+        <v>0.768202657807309</v>
       </c>
       <c r="E104" t="n">
-        <v>0.7405238095238095</v>
+        <v>0.768202657807309</v>
       </c>
     </row>
     <row r="105">
@@ -2419,13 +2419,13 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.4696896860924157</v>
+        <v>0.4987368946012383</v>
       </c>
       <c r="C105" t="n">
-        <v>0.4368215695802792</v>
+        <v>0.4219038048670982</v>
       </c>
       <c r="D105" t="n">
-        <v>0.4207601668390572</v>
+        <v>0.4191674266477046</v>
       </c>
       <c r="E105" t="n">
         <v>903000</v>
@@ -2438,13 +2438,13 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.7370964910024791</v>
+        <v>0.8104317137722559</v>
       </c>
       <c r="C106" t="n">
-        <v>0.7405238095238095</v>
+        <v>0.768202657807309</v>
       </c>
       <c r="D106" t="n">
-        <v>0.7237812208396108</v>
+        <v>0.7528114588982721</v>
       </c>
       <c r="E106" t="n">
         <v>903000</v>

</xml_diff>